<commit_message>
Slight Changes in Work Schedule
</commit_message>
<xml_diff>
--- a/Work Schedule.xlsx
+++ b/Work Schedule.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -52,8 +52,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -81,9 +89,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -93,6 +102,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -141,7 +153,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -176,7 +188,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -388,7 +400,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,16 +412,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -438,7 +450,7 @@
         <v>43348</v>
       </c>
       <c r="D3" s="1">
-        <v>43256</v>
+        <v>43348</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -449,7 +461,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="1">
-        <v>43256</v>
+        <v>43348</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -460,11 +472,12 @@
         <v>5</v>
       </c>
       <c r="C5" s="1">
-        <v>43256</v>
+        <v>43348</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
committed by swaroop Acharjee 1:09pm 05/09/18
</commit_message>
<xml_diff>
--- a/Work Schedule.xlsx
+++ b/Work Schedule.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>To do</t>
   </si>
@@ -37,6 +37,15 @@
   </si>
   <si>
     <t>Career Blog backend framework</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Rudrajit Bhattacharya</t>
+  </si>
+  <si>
+    <t>Each of the Article Page</t>
   </si>
 </sst>
 </file>
@@ -376,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,6 +423,9 @@
       <c r="C2" s="1">
         <v>43348</v>
       </c>
+      <c r="D2" s="1">
+        <v>43348</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -424,6 +436,31 @@
       </c>
       <c r="C3" s="1">
         <v>43348</v>
+      </c>
+      <c r="D3" s="1">
+        <v>43256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1">
+        <v>43256</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>43256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
committed by Swaroop Acharjee 06-09-2018 1:40am
</commit_message>
<xml_diff>
--- a/Work Schedule.xlsx
+++ b/Work Schedule.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t>To do</t>
   </si>
@@ -46,6 +46,60 @@
   </si>
   <si>
     <t>Each of the Article Page</t>
+  </si>
+  <si>
+    <t>Fixing the UI of the each Blog page</t>
+  </si>
+  <si>
+    <t>Getting the time required to read the article</t>
+  </si>
+  <si>
+    <t>Header Image of each of the blog required</t>
+  </si>
+  <si>
+    <t>Social Sharing Option for each of the blog</t>
+  </si>
+  <si>
+    <t>Creating Model Class for each of the blog article</t>
+  </si>
+  <si>
+    <t>DB support for the author and links</t>
+  </si>
+  <si>
+    <t>Suggested Reads</t>
+  </si>
+  <si>
+    <t>Navigation Bar for the Blog</t>
+  </si>
+  <si>
+    <t>Footer Bar for the blog</t>
+  </si>
+  <si>
+    <t>Font of the blog</t>
+  </si>
+  <si>
+    <t>Deciding on the Color Scheme of the Blog</t>
+  </si>
+  <si>
+    <t>Anchor List in the blog</t>
+  </si>
+  <si>
+    <t>Sprint 1 (IMPROVING THE LOOK AND FEEL OF THE  EACH OF THE BLOG POST)</t>
+  </si>
+  <si>
+    <t>Shradha/Rudrajit/Ankit</t>
+  </si>
+  <si>
+    <t>Demographic Test</t>
+  </si>
+  <si>
+    <t>All team</t>
+  </si>
+  <si>
+    <t>Approval of Code</t>
+  </si>
+  <si>
+    <t>Sprint 2 (IMPROVING THE LOOK AND FEEL OF HOME PAGE OF THE CAREER BLOG)</t>
   </si>
 </sst>
 </file>
@@ -61,12 +115,54 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -81,9 +177,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,8 +568,178 @@
         <v>43256</v>
       </c>
     </row>
+    <row r="6" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>43349</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1">
+        <v>43349</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1">
+        <v>43349</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="9">
+        <v>43349</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1">
+        <v>43349</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1">
+        <v>43349</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1">
+        <v>43349</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1">
+        <v>43349</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1">
+        <v>43349</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="1">
+        <v>43349</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="1">
+        <v>43349</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1">
+        <v>43349</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="1">
+        <v>43349</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="1">
+        <v>43349</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>